<commit_message>
Made some file changes
</commit_message>
<xml_diff>
--- a/WebApplication1/issues.xlsx
+++ b/WebApplication1/issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nirav\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8183B43-983B-4292-BC30-2387F0C7EF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829A658F-AEAB-4A3E-8333-21337A0FA541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1290" yWindow="-110" windowWidth="18020" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>IssueID</t>
   </si>
@@ -34,49 +34,37 @@
     <t>Solution</t>
   </si>
   <si>
-    <t>An item I ordered</t>
-  </si>
-  <si>
-    <t>Tevlaphee Steering Wheel Lock</t>
-  </si>
-  <si>
-    <t>Yes, help me return</t>
-  </si>
-  <si>
-    <t>No, something else</t>
-  </si>
-  <si>
-    <t>Got it. What do you need help with?</t>
-  </si>
-  <si>
-    <t>Managing my account</t>
-  </si>
-  <si>
-    <t>Kindle, Fire, or Amazon device</t>
-  </si>
-  <si>
-    <t>Music, eBooks, Prime Video, etc.</t>
-  </si>
-  <si>
-    <t>An unknown charge</t>
-  </si>
-  <si>
-    <t>We can help you manage account details here.</t>
-  </si>
-  <si>
-    <t>We support Kindle and Fire troubleshooting.</t>
-  </si>
-  <si>
-    <t>Support for digital content issues.</t>
-  </si>
-  <si>
-    <t>Check your account billing history.</t>
-  </si>
-  <si>
-    <t>We've started your return. You’ll get an email soon.</t>
-  </si>
-  <si>
-    <t>Iphone 16 256 GB</t>
+    <t>Payment Issues</t>
+  </si>
+  <si>
+    <t>Refund for Cancelled Order</t>
+  </si>
+  <si>
+    <t>Failed Payment Retry</t>
+  </si>
+  <si>
+    <t>Report Issues</t>
+  </si>
+  <si>
+    <t>Report Order Issue</t>
+  </si>
+  <si>
+    <t>Delayed Shipment</t>
+  </si>
+  <si>
+    <t>Submit refund request via support form.</t>
+  </si>
+  <si>
+    <t>Try using a different payment method.</t>
+  </si>
+  <si>
+    <t>Email support with your order number.</t>
+  </si>
+  <si>
+    <t>Track shipment via your account or contact support.</t>
+  </si>
+  <si>
+    <t>I need help with something else</t>
   </si>
 </sst>
 </file>
@@ -444,16 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="23.54296875" customWidth="1"/>
+    <col min="3" max="3" width="26.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -480,104 +467,74 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>